<commit_message>
change text column in table
</commit_message>
<xml_diff>
--- a/aspnet-core/src/ProjectManagement.Web.Host/wwwroot/template/InvoiceForTax.xlsx
+++ b/aspnet-core/src/ProjectManagement.Web.Host/wwwroot/template/InvoiceForTax.xlsx
@@ -114,9 +114,6 @@
     <t>DATE AT</t>
   </si>
   <si>
-    <t>WORKING HOUR</t>
-  </si>
-  <si>
     <t>TASK NAME</t>
   </si>
   <si>
@@ -124,6 +121,9 @@
   </si>
   <si>
     <t>TIMESHEET OF USER IN PROJECT</t>
+  </si>
+  <si>
+    <t>MAN DAY</t>
   </si>
 </sst>
 </file>
@@ -488,6 +488,27 @@
     <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -507,27 +528,6 @@
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="168" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -829,7 +829,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="InvoiceDetails4" displayName="InvoiceDetails4" ref="B3:E4" insertRow="1">
   <tableColumns count="4">
     <tableColumn id="1" name="DATE AT" dataDxfId="3"/>
-    <tableColumn id="6" name="WORKING HOUR" dataDxfId="2"/>
+    <tableColumn id="6" name="MAN DAY" dataDxfId="2"/>
     <tableColumn id="5" name="TASK NAME" dataDxfId="1"/>
     <tableColumn id="2" name="NOTE" dataDxfId="0"/>
   </tableColumns>
@@ -1071,7 +1071,7 @@
   <dimension ref="B1:K24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="H15" sqref="B14:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
@@ -1101,17 +1101,17 @@
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="2:11" ht="24" customHeight="1">
-      <c r="B3" s="51">
+      <c r="B3" s="44">
         <v>44015</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="56">
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="49">
         <f>InvoiceTotal</f>
         <v>0</v>
       </c>
-      <c r="G3" s="56"/>
+      <c r="G3" s="49"/>
       <c r="H3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1123,53 +1123,53 @@
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="7"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="57"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
       <c r="H4" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:11">
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="53" t="s">
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="53"/>
+      <c r="G6" s="46"/>
     </row>
     <row r="7" spans="2:11">
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="55" t="s">
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="55"/>
+      <c r="G7" s="48"/>
     </row>
     <row r="8" spans="2:11">
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
     </row>
     <row r="9" spans="2:11">
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
       <c r="G9" s="10"/>
     </row>
     <row r="10" spans="2:11" ht="12.75" customHeight="1">
@@ -1273,8 +1273,8 @@
       <c r="C19" s="30"/>
       <c r="D19" s="30"/>
       <c r="E19" s="30"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="49">
+      <c r="F19" s="54"/>
+      <c r="G19" s="56">
         <f>0</f>
         <v>0</v>
       </c>
@@ -1284,8 +1284,8 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="50"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="57"/>
     </row>
     <row r="22" spans="2:10" ht="15">
       <c r="B22" s="31" t="s">
@@ -1306,29 +1306,29 @@
       <c r="G23" s="33"/>
     </row>
     <row r="24" spans="2:10" ht="27" customHeight="1">
-      <c r="B24" s="44"/>
-      <c r="C24" s="44"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="44"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="44"/>
+      <c r="B24" s="51"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="51"/>
+      <c r="F24" s="51"/>
+      <c r="G24" s="51"/>
       <c r="J24" s="34"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="12">
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F3:G4"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
@@ -1344,7 +1344,7 @@
   <dimension ref="B1:F6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -1359,7 +1359,7 @@
     <row r="1" spans="2:6" ht="30.75" customHeight="1"/>
     <row r="2" spans="2:6" ht="35.25" customHeight="1">
       <c r="B2" s="58" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="58"/>
       <c r="D2" s="58"/>
@@ -1370,13 +1370,13 @@
         <v>19</v>
       </c>
       <c r="C3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="E3" s="16" t="s">
         <v>21</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>22</v>
       </c>
       <c r="F3" s="3"/>
     </row>

</xml_diff>

<commit_message>
31122 31142 31168 31032 31164
</commit_message>
<xml_diff>
--- a/aspnet-core/src/ProjectManagement.Web.Host/wwwroot/template/InvoiceForTax.xlsx
+++ b/aspnet-core/src/ProjectManagement.Web.Host/wwwroot/template/InvoiceForTax.xlsx
@@ -554,7 +554,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1093,7 +1093,7 @@
   <dimension ref="B1:K24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:I9"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>

</xml_diff>